<commit_message>
Auto commit by GitHub Action
</commit_message>
<xml_diff>
--- a/script_info.xlsx
+++ b/script_info.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="未成功爬取的脚本ID" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3986,46 +3985,4078 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>未成功爬取的脚本ID范围</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>未成功爬取的脚本ID</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>113-246</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>113,114,112,135,136,139,138,141,145,157,165,163,167,172,178,181,192,202,203,208,207,209,216,224,229,244,248,249,250,247,246</t>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>259</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Greasy Fork - Search other sites</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Add search option to search on Userscripts.org and *cough* OpenUserJS.org.</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>LouCypher</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/259</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>258</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Don't Read Below the Line</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Script intended to reduce misanthropic feelings, by hiding the comments section on some UK newspapers.</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>JynxZero</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/258</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>252</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Inoreader: enlarge images</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Replaces small Blogger, Flickr, Tumblr, and NASA Earth Observatory feed images with larger ones in Inoreader.</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>joshg253</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/252</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>253</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Inoreader: enlarge images</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Replaces small Blogger, Flickr, Tumblr, and NASA Earth Observatory feed images with larger ones in Inoreader.</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>joshg253</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/253</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>257</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Chess.com Favicon Alerts</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Add number of games waiting to favicon</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>JynxZero</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/257</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>255</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Inoreader: enlarge images</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Replaces small Blogger, Flickr, Tumblr, and NASA Earth Observatory feed images with larger ones in Inoreader.</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>joshg253</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/255</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>260</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>niconico リンクを修正</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Replaces JavaScript links with HTML links in Niconico. Also adds “Reuse” button also to also reserved broadcasts on the Nico Live My Page.</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/260</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>254</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Inoreader: enlarge images</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Replaces small Blogger, Flickr, Tumblr, and NASA Earth Observatory feed images with larger ones in Inoreader.</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>joshg253</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/254</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>256</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>LiveLeak: stretch video</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>stretch the videos on LiveLeak, hide right column</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>joshg253</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/256</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>265</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>pixiv 検索オプションを追加</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>This is a search option add-on script for pixiv. Enables you to select search mode by radio buttons (legacy feature).</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/265</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>271</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>HTMLダイアログ無効化</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Always opens JavaScript links in new tab in current window instead of new window.</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/271</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>262</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>pixiv タグクラウドからピックアップ</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Restores the tag cloud (illustration or novel tags column), and if there are tags attached to a work, this script brings those tags to the top of the tag cloud (illustration tags column).</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/262</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>264</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Drag &amp; DropZones +</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>[userChromeJS] Drag selected character strings or image and drop to the semitransparent box displayed on web page to open search result.</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/264</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>268</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Append Tag Searching Tub</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Adds “Keyword”, “Tags”, “My List”, “Images” and “Live” search tabs to all of the Niconico search boxes.</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/268</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>266</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>pixiv コメントを展開</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Expands pixiv comments. Always shows all comments (and replies).</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/266</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>267</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Bug 667607 (Fill the tab bar after closing a tab)</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>[userChromeJS] Resize tabs to fill the tab bar immediately after closing a tab (Firefox 4 feature).</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/267</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>280</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>HTML5 for MoeFM</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>萌否电台 HTML5 脚本</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/280</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>274</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Google 検索窓を複製</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Also shows the search box to the page bottom.</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/274</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>272</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>ニコ生アラート（簡）</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Alerts you to live streams that match your search. Supports these sites:  FC2 Live, SHOWROOM, Stickam JAPAN!, TwitCasting, Twitch, Niconico Live, Himawari Stream, FRESH! (AbemaTV), Whowatch, Periscope (Twitter)</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/272</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>278</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Zitate</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Versteckt überflüssige Zitate, die aber wieder einblendbar sind.</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/278</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>277</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Forennavigation - Dashboard</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Fügt der Navigationsleiste am Dashboard die fehlenden Links und Knöpfe hinzu.</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/277</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>275</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Clone Turning Page Button in nicovideo</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Also shows the pagination on the top of Nico Live search result, Lives by Category page, and Nico Video user page.</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>100の人</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/275</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>281</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>CC Code</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>CC Code 是一个贴吧扩展程序/脚本，功能类似于“度伴娘”中的贴吧小工具。</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/281</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>279</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Ignorefunktion</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Versieht das Forum mit einer einstellbaren Ignorefunktion.</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/279</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>290</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>WaniKani Review Search</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Do a WaniKani Search on your review answer.  By gth99.</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>RhosVeedcy</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/290</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>283</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Baidu Zhidao Thread Notification</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>在贴吧对来自百度知道的贴子进行提醒和删除。</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/283</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>286</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Moe-FM Downloader</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Download music when listening to the music on Moe.FM</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/286</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>282</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Tieba Preload</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>贴吧预加载，自动加载下一页内容，同时附带消灭贴吧自带 Lazy Load 功能</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/282</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>284</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Moe-FM Fav-Songs Random Play</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>随机播放萌否电台中收藏的音乐的小脚本(￣▽￣")……</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/284</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>289</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Tieba Template</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>贴吧模板</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/289</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>288</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>SearchPreview for Baidu</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>SearchPreview for Baidu 伪百度搜索预览，提供一站式服务，无页面转跳，适合快速搜索资料。Re-edit by 864907600cc</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/288</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>287</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Tieba Quick Post</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Press Ctrl + Enter to post a thread / comment on Tieba.</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/287</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>291</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>查看发帖</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>查看百度贴吧某用户在某贴吧或者全部贴吧的发言</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/291</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>285</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>伪·转换贴吧 ed2k 链接</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>将贴吧里提醒“贴吧安卓客户端可直接观看影片”的 ed2k 链接转换为可点击下载的链接……</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>864907600cc</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/285</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>299</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>quick-view-douban</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>see douban book movie music in every webpage by selecting text</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>ywzhaiqi</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/299</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>296</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>No noticeTitleFlash on BBS</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>卡饭论坛去除标题栏闪烁提醒</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>ywzhaiqi</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/296</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>300</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Douban Download Search</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>增加豆瓣电影、图书的下载搜索链接</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>ywzhaiqi</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/300</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>292</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>My Novel Reader</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>小说阅读脚本，统一阅读样式，内容去广告、修正拼音字、段落整理，自动下一页</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>ywzhaiqi</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/292</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>309</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Light Rising Tweaks</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Some minor tweaks for Light Rising browser game</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/309</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>305</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>userscripts 只显示中文</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>在 userscripts、greasyfork 脚本页面只显示中文脚本，支持 AutoPager 和其它翻页脚本。</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>ywzhaiqi</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/305</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>310</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Nexus Clash Interface Tweaks</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Various Tweaks to the Nexus Clash Browser Game Interface</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/310</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>308</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Reddit visited link remover</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>hides links you already visited on reddit and offers keyboard navigatin</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>sxe</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/308</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>311</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Light Rising AutoFuel</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Adds an 'Add Fuel 10x' button to Light Rising Browser Game</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/311</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>319</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Nexus Clash Newspaper Wiki Text</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Adds button to newspaper view thats adds wiki ready version</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/319</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>314</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Nexus Clash Recall Last Charge Attack</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>For Gunwizards. Rememebers last attack power up for arcane marksman</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/314</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>321</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Nexus Clash Default Prayer is for Magic</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Makes default prayer be for magic</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/321</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>312</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Light Rising Craft Lock</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Remember a craft or build option. Handy when getting components.</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/312</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>316</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Nexus Clash Colour Messages</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Message colour coding for Nexus Clash Browser Game</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/316</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>320</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Light Rising Crafting Checker</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Shows if any crafting tools or ingredients are missing</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/320</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>313</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Nexus Clash Stat Bars</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Adds bars to AP HP and MP</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/313</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>318</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Shintolin Tweaks</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Tweaks for Shintolin Browser Game</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/318</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>317</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Nexus Clash Forums Newspaper Wiki Text</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Trys to find and convert forum posts containing newspaper leaderboards to wiki ready text</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/317</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>315</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Nexus Clash Add Drop Item Safety Check Box</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Make it a tad harder to drop things</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/315</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>330</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Shintolin AutoSearch</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Adds Search 10x button</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/330</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>323</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Light Rising AutoQuarry</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Adds a Quarry 10X button.</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/323</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>328</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>NexusClashReadableInfusion</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Makes infusion numbers readable</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/328</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>326</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Shintolin Building Checker</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Shows if any building tools or components are missing</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/326</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>325</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Shintolin Remember Last Weapon</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Remembers last weapon used and autoselects it.</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/325</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>324</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Light Rising Remember Last Weapon</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Remembers last weapon used and autoselects it.</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/324</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>329</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Nexus Clash Remove Spell Gem Color</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>In the faction safe removes the color from spell gems and resorts them alphabetically</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/329</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>331</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Light Rising Anti Wall Climbing</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Stops accidental wall climbing.</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/331</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>322</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Light Rising Remember Number of Items</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>AutoSelects value used for number of items for Give/Drop/Take actions</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/322</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>327</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Shintolin Crafting Checker</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Shows if any crafting tools or ingredients are missing</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/327</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>338</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Shanbay message assistant</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Shanbay 短信助手</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>mozillazg</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/338</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>336</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Markdown textarea</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Add Markdown convert button to textarea</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>mozillazg</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/336</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>335</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Shartak Rearrange Inventory</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>rearranges a few inventory items</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/335</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>332</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Light Rising Building Checker</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Shows if any building tools or components are missing</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/332</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>334</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Shartak Rearrange Inventory Lite</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>rearranges a few less inventory items</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/334</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>333</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Light Rising AutoSearch</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Adds 'Search 10x' button</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Kiwimage</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/333</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>337</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Better Shanbay</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Enhance shanbay.com</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>mozillazg</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/337</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>340</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Popup Search</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Popup search box and translate button (etc) for selected texts</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>lkytal</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/340</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>350</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>iZhihu</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>知乎插件</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>unogz</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/350</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>345</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Tieba Enhance</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>贴吧小尾巴, 坟贴提醒, 去除跳转等功能</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>lkytal</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/345</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>348</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>RTCMultiConnection</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Library for comfortable using WebRTC technology.</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Kilowatt</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/348</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>349</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>qidian download</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>方便在html5起点站下载小说</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/349</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>343</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Open Discuz Link in new tab</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Discuz论坛链接默认新链接打开,支持autopager和Super_preloader等</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>lkytal</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/343</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>342</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Text To link</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Turn plain text URLs into clickable links</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>lkytal</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/342</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>351</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Dislike-Knopf</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Reaktiviert den Dislike-Knopf</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/351</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>344</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Google Image Search Context Menu</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Add Search Image context menu</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>lkytal</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/344</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>356</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Gelöscht von meinem Userscript mit Tapa-Ex</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Entfernt die nutzlosen "Gesendet von"-Texte</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/356</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>357</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>tiebaOldVersion</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>自动返回旧版贴吧</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/357</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>352</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Eishockeyforum - Links in alten Zitaten</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Repariert die alten Links in den Zitaten</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/352</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>353</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>HowrseHorseImageSwap-Frieisan</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Swaps the Friesian V4 default coat for the V3 default coat</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>daexion</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/353</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>355</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>tieba_emotion_helper</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>贴吧自定义表情批量修改</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/355</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>354</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>XuanFengEx</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>QQ旋风网页版离线下载增强</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>rhyzx</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/354</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>365</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Batoto MyFollows</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Filter your follows from comic search; info button and sorting in the old follows page; links between Batoto-MU-Mal and other features.</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>MadHero</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/365</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>370</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Stop Overzealous Embedding</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Tries to turn embedded Youtube videos into links</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Connor Behan</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/370</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>371</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Kill Floating Bars</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Stops elements from following you as you scroll down the page</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Connor Behan</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/371</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>364</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Camp-Firefox.de - Ignorefunktion</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Ignorefunktion für camp-firefox.de</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Elbart</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/364</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>368</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Gotoquiz refresh posts.</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Refresh the posts on gotoquiz forums</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>OswaldTheHatter</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/368</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>366</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Howrse Swap all v4 &gt;&gt; v3 Default Coats</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Swaps all of the v4 default coats for the v3 default coats</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>daexion</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/366</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>374</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Twitch Plays Pokemon - Command Filtering &amp; Spamming Tool</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Adds tools to your chatbox for spamming chat and filtering out commands from chat.</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>mugwhump</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/374</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>373</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Kill Typeahead Search</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Removes drop down lists that try to second guess the user</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Connor Behan</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/373</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>380</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Scrying Workshop Reworked</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>UX Improvements for Flight Rising's Scrying Workshop and Search</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>UXRising</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/380</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>372</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Expand Wikipedia Acronyms</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Provides a better tooltip for a link to a Wikipedia page about an acronym</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Connor Behan</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/372</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>375</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Newegg ComboEgger</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Automatically retrieves and displays egg ratings for all products in a Newegg ComboBundle page.</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>JamesSwift</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/375</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>387</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>HTML5 YouTube F key fullscreen</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Make YouTube's HTML5 player go fullscreen when pressing F</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>DaVince</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/387</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>388</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>HTML5 video auto-pause</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Auto-pause any HTML5 videos. Will still preload.</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>DaVince</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/388</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>385</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Swefilmer</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Wide player, and store layout to next time you change. Navigate faster to Next TV-Series or the previous one. Easy to see where you are. (colored)</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>magnus 2</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/385</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>386</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>waitUntilExists</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Is a small one function script, my most use one I use..</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>magnus 2</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/386</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>399</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Reddit-Upvoter</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Upvote all links/comments on the page</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>drakulaboy</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/399</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>398</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>TMD filtru torrente</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>ascunde torrentele care nu le doresti</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>drakulaboy</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/398</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>407</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>WM Common Library</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>A collection of useful functions and objects, some of which are specific to the Wall Manager family of scripts.</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/407</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>410</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>WM Config Interface</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Creates a configuration interface which allows users to set and get options easily.</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/410</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>408</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>WM Debug Console</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Creates a debug console that slides up from the bottom right of the screen</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/408</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>411</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>WM Graph API Interface (Beta Branch)</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Creates a low-access, read-only interface to the FB Graph API.</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/411</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>409</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>JS Forms Library B</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Encapulates and extends many HTML forms elements.</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/409</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>405</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Wall Manager Sidekick (Farmville)</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Assists Wall Manager with Farmville posts</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/405</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>406</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Mutik's DotD Script</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Fork of ForTheGoodOfAll DotD script with new look and strongly optimized js code</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>mutik</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/406</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>418</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>JS Forms Library B</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Encapulates and extends many HTML forms elements.</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/418</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>420</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>WM Graph API Interface (Beta Branch)</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Creates a low-access, read-only interface to the FB Graph API.</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/420</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>417</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>WM Debug Console</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Creates a debug console that slides up from the bottom right of the screen</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/417</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>421</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>FB Wall Manager</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Manages Wall Posts for Various FB Games</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/421</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>412</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>FB Wall Manager</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Manages Wall Posts for Various FB Games</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>thehumblesupremo</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/412</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>419</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>WM Config Interface</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Creates a configuration interface which allows users to set and get options easily.</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/419</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>416</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>WM Common Library</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>A collection of useful functions and objects, some of which are specific to the Wall Manager family of scripts.</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Merricksdad</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/416</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>430</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Tieba_Insert_MusicLink</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>贴吧自定义插入mp3链接</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/430</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>436</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>WatchWatch</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>GINZAwatchに時計復活。 ついでに過去ログ時間選択も使いやすくする</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/436</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>434</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>SmartNicorepo</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>ニコレポの「投稿」以外をデフォルトで折りたたむ</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/434</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>433</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Nico HeatMap</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>コメントの盛り上がり状態をシンプルにグラフ表示。 GINZA用</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/433</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>437</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>KeepScrollPosition</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>マイページでマイリストから削除したときにスクロール位置を保持するやつ</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/437</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>439</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>nicosJumpCanceller</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>「＠ジャンプ」を無効化</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/439</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>432</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>楼中楼回复自动加@</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>百度贴吧楼中楼回复自动加上@</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/432</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>438</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>NicoWheelVolume</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>マウスのボタン＋ホイールで、どこでも音量調整 for ニコニコ動画とYouTube</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/438</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>435</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Nicorenizer</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>動画クリックで一時停止/再開 ダブルクリックでフルスクリーン切換え</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/435</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>445</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>myTImenu - Personal version</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Create new buttons on NavTab and drop down menus on top</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Silveress</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/445</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>446</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Google Calendar Views - Personal version</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Have several calendars? Stop clicking and create views in Google's calendar application</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Silveress</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/446</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>453</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>WatchItLater</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>動画を見る前にマイリストに登録したいGreasemonkey (Chrome/Fx用)</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/453</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>461</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>QR-Plugins.TextMechanic</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>plugins for Kaskus-QR TextMechanic generator</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/461</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>460</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>QR-Plugins.RainbowText</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>plugins for Kaskus-QR rainbowtext generator</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/460</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>452</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>ShinjukuWatch</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>新しい原宿　略して新宿</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/452</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>458</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>QR-Plugins.EmbedMedia</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>plugins for Kaskus-QR embed media, eg SoundCloud, Vimeo</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/458</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>455</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>BlastarBegoner ][+</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>further enhancements for Kuro5hin.org</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Nimey</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/455</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>457</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>QR-Plugins.IMG.WrapBBCode</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>plugins for Kaskus-QR, wrap all image link with img bbcode</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/457</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>459</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>QR-Plugins.TextFliper</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>plugins for Kaskus-QR TextFliper generator</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/459</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>456</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Affiliate killer</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>No more Affiliate Link! Plz Original URL!</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>noisys</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/456</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>454</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>MOD_Seiga</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>ニコニコ静画のUIをいじる</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>segabito</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/454</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>469</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Super Bawu</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>吧务拉黑封禁功能增强</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/469</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>467</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Github Commit Whitespace</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Adds button to hide whitespaces from commit</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>jerone</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/467</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>466</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Outlook Sign Out To Login</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Redirect back to login page when signing out from Outlook</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>jerone</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/466</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>463</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Greasyfork Require Easy Get Latest Version</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Puts the link for the latest version of a library into an input with autoselect instead of a code tag.</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Tobbe</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/463</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>465</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>GeenStijl &amp; Powned &amp; Dumpert Comment Enhancer</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Add features to enhance comments on GeenStijl &amp; Powned &amp; Dumpert &amp; more.</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>jerone</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/465</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>468</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Youtube Video Ratings TEST</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Shows the rating as well as the ratio of likes per views (Like Strength) below each video's thumbnail.</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>lednerg</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/468</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>462</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Fixed Scroller Anywhere</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>fixedscrollanywhere</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>tuxie.forte</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/462</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>473</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Kiss Insights Goodbye</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Remove KissInsights dialogs from all web sites.</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/473</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>480</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>on.js</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>A micro-library for DRY:ing up the boring boilerplate of user scripts</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/480</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>477</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Plan B: inline footnotes</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Lets you click footnotes in Earth Policy Institute's "Plan B" series of books to bring them to your eyes, rather than have you chase down the page to the reference, and back again afterward. Hypertext!</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/477</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>474</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Github: unfold commit history</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Adds "unfold all changesets" buttons (hotkey: f) above/below Commit History pages at github, letting you browse the source changes without leaving the page. (Click a commit header again to re-fold it.) You can also fold or unfold individual commits by clicking on non-link parts of the commit. As a bonus, all named commits get their tag/branch names annotated in little bubbles on the right.</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/474</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>481</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Tieba Private</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>自动清除贴吧个人主页【最近来访】记录</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>文科</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/481</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>476</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Wikipedia Inline Footnotes</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Shows footnotes inline when clicked.</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/476</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>475</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Github: JSON reformatter</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Reformats JSON(P) files in the github tree view for readability.</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>johan 2</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/475</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>490</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Hide Chess.com Opponent Ratings</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Hide ratings in games, and on your homepage.  For those who don't want a constant reminder that their opponent is better (or worse) than them.</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>JynxZero</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/490</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>485</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>pikabu: Watch Later</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Позволяет складывать загружающиеся гифки в сторону, чтобы потом не возвращаться к ним</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Kilowatt</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/485</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>489</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>百度贴吧图片缩放增强脚本</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>增强百度贴吧图片缩放，看大图无需开新标签页。</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>patwonder</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/489</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>484</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Hitbox Emotes</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>The original Hitbox Emotes script with ober 15,000 emotes! - Request your custom emotes and mod badges here!</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>GamingTom</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/484</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>488</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Ilta-Saatana Iltalehdelle</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Saatana!</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>veeti</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/488</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>487</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Ilta-Saatana Ilta-Sanomille</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Saatana!</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>veeti</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/487</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>494</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>YouTube Auto Buffer &amp; Auto HD</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Buffers the video without autoplaying and puts it in HD if the option is on. For Firefox, Opera, &amp; Chrome</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>JoeSimmons</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/494</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>492</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>AoA:GE</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Age of Aincrad: Guild Edition</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Haranobu</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/492</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>495</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Remove Chess.com User Stylesheets</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Remove custom stylesheets from group and user pages</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>JynxZero</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/495</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>499</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Soundcloud Disable Comments</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Remove comment elements from Soundcloud waveforms.</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>tim 3</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/499</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>493</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Github Comment Enhancer</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Enhances Github comments</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>jerone</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/493</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>496</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>百度云插件+APIKey</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>在百度云网盘的页面添加一个搜索框，调用搜索API搜索所有公开分享文件// To add a search frame that calls some api for searching some public shared files in BaiduYun cloud netdisk.</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>cinima</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>https://greasyfork.org/zh-CN/scripts/496</t>
         </is>
       </c>
     </row>

</xml_diff>